<commit_message>
march 1 add 3star macro
</commit_message>
<xml_diff>
--- a/pub/秘诀流分析.xlsx
+++ b/pub/秘诀流分析.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
   <si>
     <t>基准概率</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -183,118 +183,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Round</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quality</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Skill</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Situation: ~100 cp, Steady Hand remains 2 rounds</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Steady H</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heart of Crafter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trick</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Great S</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ingen II</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Byregot</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trick</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CS II</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SH ends</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hasty T</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Byregot</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Steady H</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Great S</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ingen II</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>51 Mythrite</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -326,6 +214,94 @@
   </si>
   <si>
     <t>Good within GS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态: ~100 cp, 稳手还有2回合</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>品质</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>品质</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>工匠之魂</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>秘诀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>高品质</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓促</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>秘诀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>阔步</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新颖II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>模范II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>阔步</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新颖II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳手结束</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1606,11 +1582,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="405633040"/>
-        <c:axId val="405627056"/>
+        <c:axId val="-1278788032"/>
+        <c:axId val="-1278778784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="405633040"/>
+        <c:axId val="-1278788032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1647,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405627056"/>
+        <c:crossAx val="-1278778784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1679,7 +1655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="405627056"/>
+        <c:axId val="-1278778784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1741,7 +1717,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405633040"/>
+        <c:crossAx val="-1278788032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2189,8 +2165,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="51"/>
-        <c:axId val="405635216"/>
-        <c:axId val="405636304"/>
+        <c:axId val="-1278776608"/>
+        <c:axId val="-1278786944"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2290,7 +2266,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="405635216"/>
+        <c:axId val="-1278776608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2333,7 +2309,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405636304"/>
+        <c:crossAx val="-1278786944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2341,7 +2317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="405636304"/>
+        <c:axId val="-1278786944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2365,7 +2341,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="405635216"/>
+        <c:crossAx val="-1278776608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2535,7 +2511,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2703,7 +2678,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2815,8 +2789,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="51"/>
-        <c:axId val="193216272"/>
-        <c:axId val="193218992"/>
+        <c:axId val="-1479850976"/>
+        <c:axId val="-1210130272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2916,7 +2890,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193216272"/>
+        <c:axId val="-1479850976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2959,7 +2933,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193218992"/>
+        <c:crossAx val="-1210130272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2967,7 +2941,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193218992"/>
+        <c:axId val="-1210130272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2991,7 +2965,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193216272"/>
+        <c:crossAx val="-1479850976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3005,7 +2979,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4776,15 +4749,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>204787</xdr:rowOff>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5470,7 +5443,7 @@
   </sheetPr>
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9004,7 +8977,7 @@
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.75" defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9016,12 +8989,12 @@
   <sheetData>
     <row r="1" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="31" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="47" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C3" s="47">
         <v>0</v>
@@ -9050,28 +9023,28 @@
     </row>
     <row r="4" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="47" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J4" s="47" t="s">
         <v>53</v>
@@ -9079,42 +9052,42 @@
     </row>
     <row r="5" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="47" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G5" s="49" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="H5" s="49" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="47"/>
       <c r="D6" s="31" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="47" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C7" s="47">
         <v>0</v>
@@ -9143,60 +9116,60 @@
     </row>
     <row r="8" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="47" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G8" s="50" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J8" s="50" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="47" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F9" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="49" t="s">
+      <c r="I9" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="49" t="s">
-        <v>63</v>
-      </c>
       <c r="J9" s="48" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -9213,7 +9186,7 @@
   </sheetPr>
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -9258,12 +9231,12 @@
         <v>31</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="K1" s="20"/>
       <c r="L1" s="53"/>
       <c r="M1" s="24" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="N1" s="20"/>
     </row>
@@ -9282,24 +9255,24 @@
       <c r="H2" s="38"/>
       <c r="I2" s="22"/>
       <c r="J2" s="25" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="K2" s="25">
         <f>COUNT(A4:A110)</f>
         <v>41</v>
       </c>
       <c r="L2" s="54" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="N2" s="25">
         <f>COUNT(E4:E110)</f>
         <v>40</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9329,7 +9302,7 @@
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="30" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="K3" s="28">
         <f>AVERAGE(D4:D110)</f>
@@ -9340,7 +9313,7 @@
         <v>0.64459839435643906</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="N3" s="28">
         <f>AVERAGE(H4:H110)</f>
@@ -9384,7 +9357,7 @@
       </c>
       <c r="I4" s="26"/>
       <c r="J4" s="30" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="K4" s="28">
         <f>(11-AVERAGE(A4:A110))/$B$1</f>
@@ -9392,7 +9365,7 @@
       </c>
       <c r="L4" s="54"/>
       <c r="M4" s="30" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="N4" s="28">
         <f>(11-AVERAGE(E4:E110))/$B$1</f>
@@ -9791,10 +9764,10 @@
         <v>15</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>